<commit_message>
add data in testdata file
</commit_message>
<xml_diff>
--- a/target/classes/com/tutorialsninja/qa/testdata/TutorialsninjaTestData.xlsx
+++ b/target/classes/com/tutorialsninja/qa/testdata/TutorialsninjaTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Project\HybridTestNGFrameWork\src\main\java\com\tutorialsninja\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naveen pal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BD5DC4-46E1-4634-B7D6-E370DC141F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B07D99-AB27-4791-A1E2-5C585CFD0884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{B22C0EB4-B418-48C6-BDEF-AD98DF7CA467}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B22C0EB4-B418-48C6-BDEF-AD98DF7CA467}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -49,6 +49,9 @@
     <t>navi2@gmail.com</t>
   </si>
   <si>
+    <t>navi3@gmail.com</t>
+  </si>
+  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -74,12 +77,6 @@
   </si>
   <si>
     <t>arupal@gmail.com</t>
-  </si>
-  <si>
-    <t>navi3@gmail.com</t>
-  </si>
-  <si>
-    <t>navi4@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -457,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE18B70-1D95-4DEF-B7D9-BE9D692C81EE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +475,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>12345</v>
@@ -486,7 +483,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>12345</v>
@@ -494,17 +491,9 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
         <v>12345</v>
       </c>
     </row>
@@ -513,42 +502,40 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{01C7EE08-F9A3-4C5E-857C-A39202AB8C24}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{30A0ED50-E012-4FCF-8400-B33E80EEF883}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{370770F7-3BE1-4765-9614-70CEB2C7A53B}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{F038E0C7-EB63-4F96-B4F6-DF7C4E63E996}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE87121-64F6-4D5D-9993-83454420DF14}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47435347-3E48-4ACE-9A91-42001D085570}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="32.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -556,13 +543,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>999111</v>
@@ -573,13 +560,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>999222</v>
@@ -590,10 +577,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{A2388BDF-B49C-42FF-8A81-2B7875607163}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{FE796A3C-740D-49C9-8DDB-AEC615AA4638}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{26EDDC88-01AA-4B34-B2F7-ECF50341B9D9}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{DB9A7BC5-2F54-46A1-98D1-7F1168A8592A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>